<commit_message>
voltage of nodes calculated
</commit_message>
<xml_diff>
--- a/data/table.xlsx
+++ b/data/table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1198,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>